<commit_message>
Changed from RandomForestRegressor to LinearRegression
RandomForestRegressor seemed not good enough, therefore change to LinearRegression which is much better
</commit_message>
<xml_diff>
--- a/Football match predictions/Predictions/Predictions.xlsx
+++ b/Football match predictions/Predictions/Predictions.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsl\Documents\Privé\Data Analysis\Football-match-predictions\Football match predictions\Predictions\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4168BC6-85DA-4AB8-B4FE-12B5E04CF5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Home</t>
   </si>
@@ -116,9 +110,6 @@
   </si>
   <si>
     <t>France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denmark </t>
   </si>
   <si>
     <t>England</t>
@@ -133,8 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,21 +188,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +232,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -283,7 +266,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -318,10 +300,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,16 +475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -546,7 +525,7 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -558,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -567,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -581,10 +560,10 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -593,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H3">
         <v>-1</v>
@@ -602,13 +581,13 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -616,10 +595,10 @@
         <v>23</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -643,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -651,10 +630,10 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -678,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -713,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -721,10 +700,10 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -733,30 +712,30 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -783,18 +762,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -803,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -812,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -826,10 +805,10 @@
         <v>26</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -853,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -861,7 +840,7 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -873,22 +852,22 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H11">
         <v>-1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -899,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -908,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -917,24 +896,24 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -949,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -958,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -966,7 +945,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -978,7 +957,7 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -987,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1001,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1013,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1022,13 +1001,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1036,10 +1015,10 @@
         <v>29</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1048,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1063,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1050,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1083,33 +1062,33 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1118,7 +1097,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1133,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1141,10 +1120,10 @@
         <v>14</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1168,18 +1147,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1188,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H20">
         <v>-1</v>
@@ -1197,13 +1176,13 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1214,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1223,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="G21">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>-1</v>
@@ -1232,13 +1211,13 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1246,10 +1225,10 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1258,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1267,24 +1246,24 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1308,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1316,10 +1295,10 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1331,19 +1310,19 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1354,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1363,28 +1342,34 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="G26">
         <v>0</v>
       </c>
@@ -1401,13 +1386,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
@@ -1424,13 +1415,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="G28">
         <v>0</v>
       </c>
@@ -1447,13 +1444,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>14</v>
       </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
       <c r="G29">
         <v>0</v>
       </c>
@@ -1470,15 +1473,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1487,21 +1496,27 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
       </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
       <c r="G31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1510,19 +1525,25 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="G32">
         <v>0</v>
       </c>
@@ -1539,13 +1560,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
       </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="G33">
         <v>0</v>
       </c>
@@ -1562,13 +1589,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
       </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
       <c r="G34">
         <v>0</v>
       </c>
@@ -1585,15 +1618,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
       </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="G35">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1602,21 +1641,27 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
       </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
       <c r="G36">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1625,21 +1670,27 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
       </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1648,13 +1699,13 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="G38">
         <v>0</v>
       </c>
@@ -1671,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="G39">
         <v>0</v>
       </c>
@@ -1688,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="G40">
         <v>0</v>
       </c>
@@ -1705,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="G41">
         <v>0</v>
       </c>
@@ -1722,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="G42">
         <v>0</v>
       </c>
@@ -1739,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="G43">
         <v>0</v>
       </c>
@@ -1756,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="G44">
         <v>0</v>
       </c>
@@ -1773,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="G45">
         <v>0</v>
       </c>
@@ -1790,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="G46">
         <v>0</v>
       </c>
@@ -1807,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="G47">
         <v>0</v>
       </c>
@@ -1824,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="G48">
         <v>0</v>
       </c>
@@ -1841,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:11">
       <c r="G49">
         <v>0</v>
       </c>
@@ -1858,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:11">
       <c r="G50">
         <v>0</v>
       </c>
@@ -1875,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:11">
       <c r="G51">
         <v>0</v>
       </c>
@@ -1892,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:11">
       <c r="G52">
         <v>0</v>
       </c>

</xml_diff>